<commit_message>
Work for the Auto populated rental activity
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate_SRAT.xlsx
+++ b/src/main/resources/dataCreate/DataCreate_SRAT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="5430" windowWidth="15375" windowHeight="7875" activeTab="3"/>
+    <workbookView xWindow="5310" yWindow="5880" windowWidth="15375" windowHeight="7875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4235" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4296" uniqueCount="341">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -1015,6 +1015,36 @@
   </si>
   <si>
     <t>Reg2ndRevExSp4168</t>
+  </si>
+  <si>
+    <t>baseAmount</t>
+  </si>
+  <si>
+    <t>percentIncrease</t>
+  </si>
+  <si>
+    <t>calFrequency</t>
+  </si>
+  <si>
+    <t>rentalActivity</t>
+  </si>
+  <si>
+    <t>Auto-Populate</t>
+  </si>
+  <si>
+    <t>6624170</t>
+  </si>
+  <si>
+    <t>Reg2ndRevEx4170</t>
+  </si>
+  <si>
+    <t>Reg2ndRevExSp4170</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>AutoPopulateRA</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1655,15 +1685,19 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1700,13 +1734,18 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2022,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB988"/>
+  <dimension ref="A1:AA988"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2034,19 +2073,26 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1"/>
-    <col min="6" max="7" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="11" width="21.28515625" customWidth="1"/>
-    <col min="12" max="14" width="14.42578125" customWidth="1"/>
+    <col min="12" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="155" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" customWidth="1"/>
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
-    <col min="18" max="28" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
+    <col min="23" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:27">
       <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
@@ -2083,10 +2129,10 @@
       <c r="L1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="148" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="129" t="s">
+      <c r="N1" s="9" t="s">
         <v>325</v>
       </c>
       <c r="O1" s="12" t="s">
@@ -2101,18 +2147,25 @@
       <c r="R1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
+      <c r="S1" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>334</v>
+      </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-    </row>
-    <row r="2" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="49" t="s">
         <v>58</v>
       </c>
@@ -2147,7 +2200,7 @@
       <c r="M2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="25"/>
+      <c r="N2" s="151"/>
       <c r="O2" s="25" t="s">
         <v>50</v>
       </c>
@@ -2161,7 +2214,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="3" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="47" t="s">
         <v>55</v>
       </c>
@@ -2196,7 +2249,7 @@
       <c r="M3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="25"/>
+      <c r="N3" s="151"/>
       <c r="O3" s="25" t="s">
         <v>50</v>
       </c>
@@ -2210,7 +2263,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="47" t="s">
         <v>69</v>
       </c>
@@ -2245,7 +2298,7 @@
       <c r="M4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="25"/>
+      <c r="N4" s="151"/>
       <c r="O4" s="25" t="s">
         <v>50</v>
       </c>
@@ -2259,7 +2312,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="20" t="s">
         <v>70</v>
       </c>
@@ -2294,7 +2347,7 @@
       <c r="M5" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="25"/>
+      <c r="N5" s="151"/>
       <c r="O5" s="25" t="s">
         <v>50</v>
       </c>
@@ -2308,7 +2361,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="44">
         <v>6530957</v>
       </c>
@@ -2343,7 +2396,7 @@
       <c r="M6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="25"/>
+      <c r="N6" s="151"/>
       <c r="O6" s="25" t="s">
         <v>50</v>
       </c>
@@ -2357,7 +2410,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="44">
         <v>6530958</v>
       </c>
@@ -2392,7 +2445,7 @@
       <c r="M7" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="25"/>
+      <c r="N7" s="151"/>
       <c r="O7" s="25" t="s">
         <v>50</v>
       </c>
@@ -2406,7 +2459,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="20" t="s">
         <v>72</v>
       </c>
@@ -2441,7 +2494,7 @@
       <c r="M8" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="25"/>
+      <c r="N8" s="151"/>
       <c r="O8" s="25" t="s">
         <v>50</v>
       </c>
@@ -2455,7 +2508,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="9" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="48" t="s">
         <v>73</v>
       </c>
@@ -2490,7 +2543,7 @@
       <c r="M9" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="25"/>
+      <c r="N9" s="151"/>
       <c r="O9" s="25" t="s">
         <v>50</v>
       </c>
@@ -2504,7 +2557,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="44">
         <v>6551796</v>
       </c>
@@ -2539,7 +2592,7 @@
       <c r="M10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="25"/>
+      <c r="N10" s="151"/>
       <c r="O10" s="25" t="s">
         <v>50</v>
       </c>
@@ -2553,7 +2606,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:27" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="45">
         <v>6551803</v>
       </c>
@@ -2587,7 +2640,7 @@
       <c r="M11" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="25"/>
+      <c r="N11" s="151"/>
       <c r="O11" s="25" t="s">
         <v>50</v>
       </c>
@@ -2601,7 +2654,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1">
+    <row r="12" spans="1:27" ht="15" customHeight="1">
       <c r="A12" s="44">
         <v>6555587</v>
       </c>
@@ -2636,7 +2689,7 @@
       <c r="M12" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="11"/>
+      <c r="N12" s="152"/>
       <c r="O12" s="11" t="s">
         <v>50</v>
       </c>
@@ -2650,7 +2703,7 @@
         <v>201534</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1">
+    <row r="13" spans="1:27" ht="15" customHeight="1">
       <c r="A13" s="44">
         <v>6555588</v>
       </c>
@@ -2685,7 +2738,7 @@
       <c r="M13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="11"/>
+      <c r="N13" s="152"/>
       <c r="O13" s="11" t="s">
         <v>50</v>
       </c>
@@ -2699,7 +2752,7 @@
         <v>201534</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1">
+    <row r="14" spans="1:27" ht="15" customHeight="1">
       <c r="A14" s="44">
         <v>6530927</v>
       </c>
@@ -2734,7 +2787,7 @@
       <c r="M14" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N14" s="11"/>
+      <c r="N14" s="152"/>
       <c r="O14" s="11" t="s">
         <v>50</v>
       </c>
@@ -2748,7 +2801,7 @@
         <v>201534</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1">
+    <row r="15" spans="1:27" ht="15" customHeight="1">
       <c r="A15" s="44">
         <v>6530966</v>
       </c>
@@ -2783,7 +2836,7 @@
       <c r="M15" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="11"/>
+      <c r="N15" s="152"/>
       <c r="O15" s="11" t="s">
         <v>50</v>
       </c>
@@ -2797,7 +2850,7 @@
         <v>201534</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1">
+    <row r="16" spans="1:27" ht="15" customHeight="1">
       <c r="A16" s="44">
         <v>6530960</v>
       </c>
@@ -2832,7 +2885,7 @@
       <c r="M16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N16" s="11"/>
+      <c r="N16" s="152"/>
       <c r="O16" s="11" t="s">
         <v>50</v>
       </c>
@@ -2881,7 +2934,7 @@
       <c r="M17" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N17" s="11"/>
+      <c r="N17" s="152"/>
       <c r="O17" s="11" t="s">
         <v>50</v>
       </c>
@@ -2930,7 +2983,7 @@
       <c r="M18" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N18" s="11"/>
+      <c r="N18" s="152"/>
       <c r="O18" s="11" t="s">
         <v>50</v>
       </c>
@@ -2979,7 +3032,7 @@
       <c r="M19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N19" s="11"/>
+      <c r="N19" s="152"/>
       <c r="O19" s="11" t="s">
         <v>50</v>
       </c>
@@ -3028,7 +3081,7 @@
       <c r="M20" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N20" s="11"/>
+      <c r="N20" s="152"/>
       <c r="O20" s="11" t="s">
         <v>50</v>
       </c>
@@ -3076,7 +3129,7 @@
       <c r="M21" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="N21" s="11"/>
+      <c r="N21" s="152"/>
       <c r="O21" s="11" t="s">
         <v>50</v>
       </c>
@@ -3123,11 +3176,11 @@
       <c r="L22" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M22" s="34" t="s">
+      <c r="M22" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N22" s="34"/>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P22" s="57" t="s">
@@ -3173,11 +3226,11 @@
       <c r="L23" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N23" s="34"/>
-      <c r="O23" s="34" t="s">
+      <c r="O23" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P23" s="57" t="s">
@@ -3223,11 +3276,11 @@
       <c r="L24" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N24" s="34"/>
-      <c r="O24" s="34" t="s">
+      <c r="O24" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P24" s="57" t="s">
@@ -3273,11 +3326,11 @@
       <c r="L25" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N25" s="34"/>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P25" s="57" t="s">
@@ -3323,11 +3376,11 @@
       <c r="L26" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M26" s="34" t="s">
+      <c r="M26" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N26" s="34"/>
-      <c r="O26" s="34" t="s">
+      <c r="O26" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P26" s="57" t="s">
@@ -3373,11 +3426,11 @@
       <c r="L27" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M27" s="34" t="s">
+      <c r="M27" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N27" s="34"/>
-      <c r="O27" s="34" t="s">
+      <c r="O27" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P27" s="57" t="s">
@@ -3423,11 +3476,11 @@
       <c r="L28" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M28" s="34" t="s">
+      <c r="M28" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N28" s="34"/>
-      <c r="O28" s="34" t="s">
+      <c r="O28" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P28" s="57" t="s">
@@ -3473,11 +3526,11 @@
       <c r="L29" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M29" s="34" t="s">
+      <c r="M29" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N29" s="34"/>
-      <c r="O29" s="34" t="s">
+      <c r="O29" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P29" s="57" t="s">
@@ -3523,11 +3576,11 @@
       <c r="L30" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M30" s="34" t="s">
+      <c r="M30" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N30" s="34"/>
-      <c r="O30" s="34" t="s">
+      <c r="O30" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P30" s="57" t="s">
@@ -3573,11 +3626,11 @@
       <c r="L31" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M31" s="34" t="s">
+      <c r="M31" s="149" t="s">
         <v>85</v>
       </c>
       <c r="N31" s="34"/>
-      <c r="O31" s="34" t="s">
+      <c r="O31" s="150" t="s">
         <v>50</v>
       </c>
       <c r="P31" s="57" t="s">
@@ -3592,21 +3645,21 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A32" s="112"/>
-      <c r="B32" s="132" t="s">
+      <c r="B32" s="136" t="s">
         <v>229</v>
       </c>
-      <c r="C32" s="133"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="133"/>
-      <c r="F32" s="133"/>
-      <c r="G32" s="133"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="137"/>
+      <c r="E32" s="137"/>
+      <c r="F32" s="137"/>
+      <c r="G32" s="137"/>
       <c r="H32" s="59"/>
       <c r="I32" s="59"/>
       <c r="J32" s="59"/>
       <c r="K32" s="59"/>
       <c r="L32" s="59"/>
       <c r="M32" s="59"/>
-      <c r="N32" s="59"/>
+      <c r="N32" s="153"/>
       <c r="O32" s="59"/>
       <c r="P32" s="57" t="s">
         <v>201</v>
@@ -3650,7 +3703,7 @@
       <c r="M33" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N33" s="53"/>
+      <c r="N33" s="154"/>
       <c r="O33" s="53" t="s">
         <v>50</v>
       </c>
@@ -3700,7 +3753,7 @@
       <c r="M34" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N34" s="53"/>
+      <c r="N34" s="154"/>
       <c r="O34" s="53" t="s">
         <v>50</v>
       </c>
@@ -3750,7 +3803,7 @@
       <c r="M35" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N35" s="53"/>
+      <c r="N35" s="154"/>
       <c r="O35" s="53" t="s">
         <v>50</v>
       </c>
@@ -3800,7 +3853,7 @@
       <c r="M36" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N36" s="53"/>
+      <c r="N36" s="154"/>
       <c r="O36" s="53" t="s">
         <v>50</v>
       </c>
@@ -3828,7 +3881,7 @@
       <c r="K37" s="22"/>
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
+      <c r="N37" s="151"/>
       <c r="O37" s="25"/>
       <c r="P37" s="57" t="s">
         <v>201</v>
@@ -3872,7 +3925,7 @@
       <c r="M38" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N38" s="53"/>
+      <c r="N38" s="154"/>
       <c r="O38" s="53" t="s">
         <v>50</v>
       </c>
@@ -3922,7 +3975,7 @@
       <c r="M39" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N39" s="53"/>
+      <c r="N39" s="154"/>
       <c r="O39" s="53" t="s">
         <v>50</v>
       </c>
@@ -3972,7 +4025,7 @@
       <c r="M40" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N40" s="53"/>
+      <c r="N40" s="154"/>
       <c r="O40" s="53" t="s">
         <v>50</v>
       </c>
@@ -4022,7 +4075,7 @@
       <c r="M41" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N41" s="53"/>
+      <c r="N41" s="154"/>
       <c r="O41" s="53" t="s">
         <v>50</v>
       </c>
@@ -4072,7 +4125,7 @@
       <c r="M42" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N42" s="53"/>
+      <c r="N42" s="154"/>
       <c r="O42" s="53" t="s">
         <v>50</v>
       </c>
@@ -4122,7 +4175,7 @@
       <c r="M43" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N43" s="53"/>
+      <c r="N43" s="154"/>
       <c r="O43" s="53" t="s">
         <v>50</v>
       </c>
@@ -4172,7 +4225,7 @@
       <c r="M44" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N44" s="53"/>
+      <c r="N44" s="154"/>
       <c r="O44" s="53" t="s">
         <v>50</v>
       </c>
@@ -4222,7 +4275,7 @@
       <c r="M45" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N45" s="53"/>
+      <c r="N45" s="154"/>
       <c r="O45" s="53" t="s">
         <v>50</v>
       </c>
@@ -4238,21 +4291,21 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A46" s="112"/>
-      <c r="B46" s="132" t="s">
+      <c r="B46" s="136" t="s">
         <v>204</v>
       </c>
-      <c r="C46" s="133"/>
-      <c r="D46" s="133"/>
-      <c r="E46" s="133"/>
-      <c r="F46" s="133"/>
-      <c r="G46" s="133"/>
+      <c r="C46" s="137"/>
+      <c r="D46" s="137"/>
+      <c r="E46" s="137"/>
+      <c r="F46" s="137"/>
+      <c r="G46" s="137"/>
       <c r="H46" s="59"/>
       <c r="I46" s="59"/>
       <c r="J46" s="59"/>
       <c r="K46" s="59"/>
       <c r="L46" s="59"/>
       <c r="M46" s="59"/>
-      <c r="N46" s="59"/>
+      <c r="N46" s="153"/>
       <c r="O46" s="59"/>
       <c r="P46" s="57" t="s">
         <v>201</v>
@@ -4296,7 +4349,7 @@
       <c r="M47" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N47" s="53"/>
+      <c r="N47" s="154"/>
       <c r="O47" s="53" t="s">
         <v>50</v>
       </c>
@@ -4346,7 +4399,7 @@
       <c r="M48" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N48" s="53"/>
+      <c r="N48" s="154"/>
       <c r="O48" s="53" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4449,7 @@
       <c r="M49" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N49" s="53"/>
+      <c r="N49" s="154"/>
       <c r="O49" s="53" t="s">
         <v>50</v>
       </c>
@@ -4446,7 +4499,7 @@
       <c r="M50" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N50" s="53"/>
+      <c r="N50" s="154"/>
       <c r="O50" s="53" t="s">
         <v>50</v>
       </c>
@@ -4501,7 +4554,7 @@
       <c r="M52" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N52" s="53"/>
+      <c r="N52" s="154"/>
       <c r="O52" s="53" t="s">
         <v>50</v>
       </c>
@@ -4551,7 +4604,7 @@
       <c r="M53" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N53" s="53"/>
+      <c r="N53" s="154"/>
       <c r="O53" s="53" t="s">
         <v>50</v>
       </c>
@@ -4601,7 +4654,7 @@
       <c r="M54" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N54" s="53"/>
+      <c r="N54" s="154"/>
       <c r="O54" s="53" t="s">
         <v>50</v>
       </c>
@@ -4651,7 +4704,7 @@
       <c r="M55" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N55" s="53"/>
+      <c r="N55" s="154"/>
       <c r="O55" s="53" t="s">
         <v>50</v>
       </c>
@@ -4706,7 +4759,7 @@
       <c r="M57" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N57" s="53"/>
+      <c r="N57" s="154"/>
       <c r="O57" s="53" t="s">
         <v>50</v>
       </c>
@@ -4756,7 +4809,7 @@
       <c r="M58" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N58" s="53"/>
+      <c r="N58" s="154"/>
       <c r="O58" s="53" t="s">
         <v>50</v>
       </c>
@@ -4806,7 +4859,7 @@
       <c r="M59" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N59" s="53"/>
+      <c r="N59" s="154"/>
       <c r="O59" s="53" t="s">
         <v>50</v>
       </c>
@@ -4856,7 +4909,7 @@
       <c r="M60" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N60" s="53"/>
+      <c r="N60" s="154"/>
       <c r="O60" s="53" t="s">
         <v>50</v>
       </c>
@@ -4877,14 +4930,15 @@
     </row>
     <row r="62" spans="1:18" s="101" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A62" s="110"/>
-      <c r="B62" s="134" t="s">
+      <c r="B62" s="138" t="s">
         <v>259</v>
       </c>
-      <c r="C62" s="135"/>
-      <c r="D62" s="135"/>
-      <c r="E62" s="135"/>
-      <c r="F62" s="135"/>
-      <c r="G62" s="135"/>
+      <c r="C62" s="139"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="139"/>
+      <c r="F62" s="139"/>
+      <c r="G62" s="139"/>
+      <c r="N62" s="100"/>
       <c r="P62" s="57" t="s">
         <v>201</v>
       </c>
@@ -4925,7 +4979,7 @@
       <c r="M63" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N63" s="53"/>
+      <c r="N63" s="154"/>
       <c r="O63" s="53" t="s">
         <v>268</v>
       </c>
@@ -4975,7 +5029,7 @@
       <c r="M64" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N64" s="53"/>
+      <c r="N64" s="154"/>
       <c r="O64" s="53" t="s">
         <v>268</v>
       </c>
@@ -5025,7 +5079,7 @@
       <c r="M65" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N65" s="53"/>
+      <c r="N65" s="154"/>
       <c r="O65" s="53" t="s">
         <v>268</v>
       </c>
@@ -5075,7 +5129,7 @@
       <c r="M66" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N66" s="53"/>
+      <c r="N66" s="154"/>
       <c r="O66" s="53" t="s">
         <v>268</v>
       </c>
@@ -5125,7 +5179,7 @@
       <c r="M67" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N67" s="53"/>
+      <c r="N67" s="154"/>
       <c r="O67" s="53" t="s">
         <v>268</v>
       </c>
@@ -5175,7 +5229,7 @@
       <c r="M68" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N68" s="53"/>
+      <c r="N68" s="154"/>
       <c r="O68" s="53" t="s">
         <v>268</v>
       </c>
@@ -5225,7 +5279,7 @@
       <c r="M69" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N69" s="53"/>
+      <c r="N69" s="154"/>
       <c r="O69" s="53" t="s">
         <v>268</v>
       </c>
@@ -5275,7 +5329,7 @@
       <c r="M70" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N70" s="53"/>
+      <c r="N70" s="154"/>
       <c r="O70" s="53" t="s">
         <v>268</v>
       </c>
@@ -5325,7 +5379,7 @@
       <c r="M71" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N71" s="53"/>
+      <c r="N71" s="154"/>
       <c r="O71" s="53" t="s">
         <v>268</v>
       </c>
@@ -5375,7 +5429,7 @@
       <c r="M72" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N72" s="53"/>
+      <c r="N72" s="154"/>
       <c r="O72" s="53" t="s">
         <v>268</v>
       </c>
@@ -5425,7 +5479,7 @@
       <c r="M73" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N73" s="53"/>
+      <c r="N73" s="154"/>
       <c r="O73" s="53" t="s">
         <v>268</v>
       </c>
@@ -5475,7 +5529,7 @@
       <c r="M74" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N74" s="53"/>
+      <c r="N74" s="154"/>
       <c r="O74" s="53" t="s">
         <v>268</v>
       </c>
@@ -5525,7 +5579,7 @@
       <c r="M75" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N75" s="53"/>
+      <c r="N75" s="154"/>
       <c r="O75" s="53" t="s">
         <v>268</v>
       </c>
@@ -5575,7 +5629,7 @@
       <c r="M76" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N76" s="53"/>
+      <c r="N76" s="154"/>
       <c r="O76" s="53" t="s">
         <v>268</v>
       </c>
@@ -5625,7 +5679,7 @@
       <c r="M77" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N77" s="53"/>
+      <c r="N77" s="154"/>
       <c r="O77" s="53" t="s">
         <v>268</v>
       </c>
@@ -5675,7 +5729,7 @@
       <c r="M78" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N78" s="53"/>
+      <c r="N78" s="154"/>
       <c r="O78" s="53" t="s">
         <v>268</v>
       </c>
@@ -5723,7 +5777,7 @@
       <c r="M79" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="N79" s="128"/>
+      <c r="N79" s="156"/>
       <c r="O79" s="128" t="s">
         <v>268</v>
       </c>
@@ -5773,7 +5827,7 @@
       <c r="M80" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N80" s="53"/>
+      <c r="N80" s="154"/>
       <c r="O80" s="53" t="s">
         <v>268</v>
       </c>
@@ -5787,7 +5841,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="81" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A81" s="120" t="s">
         <v>300</v>
       </c>
@@ -5823,7 +5877,7 @@
       <c r="M81" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N81" s="53"/>
+      <c r="N81" s="154"/>
       <c r="O81" s="53" t="s">
         <v>268</v>
       </c>
@@ -5837,7 +5891,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="82" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A82" s="120" t="s">
         <v>301</v>
       </c>
@@ -5873,7 +5927,7 @@
       <c r="M82" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N82" s="53"/>
+      <c r="N82" s="154"/>
       <c r="O82" s="53" t="s">
         <v>268</v>
       </c>
@@ -5887,7 +5941,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="83" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A83" s="120" t="s">
         <v>302</v>
       </c>
@@ -5923,7 +5977,7 @@
       <c r="M83" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N83" s="53"/>
+      <c r="N83" s="154"/>
       <c r="O83" s="53" t="s">
         <v>268</v>
       </c>
@@ -5937,7 +5991,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="84" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A84" s="120" t="s">
         <v>303</v>
       </c>
@@ -5973,7 +6027,7 @@
       <c r="M84" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N84" s="53"/>
+      <c r="N84" s="154"/>
       <c r="O84" s="53" t="s">
         <v>268</v>
       </c>
@@ -5987,7 +6041,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="85" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A85" s="120" t="s">
         <v>304</v>
       </c>
@@ -6023,7 +6077,7 @@
       <c r="M85" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N85" s="53"/>
+      <c r="N85" s="154"/>
       <c r="O85" s="53" t="s">
         <v>268</v>
       </c>
@@ -6037,7 +6091,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="86" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A86" s="120" t="s">
         <v>305</v>
       </c>
@@ -6073,7 +6127,7 @@
       <c r="M86" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N86" s="53"/>
+      <c r="N86" s="154"/>
       <c r="O86" s="53" t="s">
         <v>268</v>
       </c>
@@ -6087,7 +6141,7 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="87" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A87" s="120"/>
       <c r="B87" s="51"/>
       <c r="C87" s="51"/>
@@ -6101,7 +6155,7 @@
       <c r="K87" s="51"/>
       <c r="L87" s="53"/>
       <c r="M87" s="53"/>
-      <c r="N87" s="53"/>
+      <c r="N87" s="154"/>
       <c r="O87" s="53"/>
       <c r="P87" s="57" t="s">
         <v>201</v>
@@ -6109,20 +6163,20 @@
       <c r="Q87" s="52"/>
       <c r="R87" s="51"/>
     </row>
-    <row r="88" spans="1:18" s="144" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="88" spans="1:22" s="131" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A88" s="119" t="s">
         <v>328</v>
       </c>
-      <c r="D88" s="145" t="s">
+      <c r="D88" s="132" t="s">
         <v>329</v>
       </c>
-      <c r="E88" s="146" t="s">
+      <c r="E88" s="133" t="s">
         <v>330</v>
       </c>
-      <c r="F88" s="147" t="s">
+      <c r="F88" s="134" t="s">
         <v>197</v>
       </c>
-      <c r="G88" s="147" t="s">
+      <c r="G88" s="134" t="s">
         <v>196</v>
       </c>
       <c r="H88" s="51" t="s">
@@ -6134,37 +6188,108 @@
       <c r="J88" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="K88" s="144" t="s">
+      <c r="K88" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="L88" s="148" t="s">
+      <c r="L88" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="M88" s="148" t="s">
+      <c r="M88" s="135" t="s">
         <v>82</v>
       </c>
-      <c r="N88" s="148"/>
-      <c r="O88" s="148" t="s">
+      <c r="N88" s="157"/>
+      <c r="O88" s="135" t="s">
         <v>268</v>
       </c>
       <c r="P88" s="74" t="s">
-        <v>54</v>
+        <v>339</v>
       </c>
       <c r="Q88" s="74" t="s">
         <v>324</v>
       </c>
-      <c r="R88" s="144">
+      <c r="R88" s="131">
         <v>201480</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="90" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="91" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="92" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="93" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="94" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="95" spans="1:18" ht="15.75" customHeight="1"/>
-    <row r="96" spans="1:18" ht="15.75" customHeight="1"/>
+      <c r="S88" s="131">
+        <v>1000</v>
+      </c>
+      <c r="T88" s="131">
+        <v>2</v>
+      </c>
+      <c r="U88" s="131">
+        <v>4</v>
+      </c>
+      <c r="V88" s="74" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" s="131" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A89" s="119" t="s">
+        <v>336</v>
+      </c>
+      <c r="D89" s="132" t="s">
+        <v>337</v>
+      </c>
+      <c r="E89" s="133" t="s">
+        <v>338</v>
+      </c>
+      <c r="F89" s="134" t="s">
+        <v>197</v>
+      </c>
+      <c r="G89" s="134" t="s">
+        <v>196</v>
+      </c>
+      <c r="H89" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="I89" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="J89" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="K89" s="131" t="s">
+        <v>36</v>
+      </c>
+      <c r="L89" s="135" t="s">
+        <v>25</v>
+      </c>
+      <c r="M89" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="N89" s="157"/>
+      <c r="O89" s="135" t="s">
+        <v>268</v>
+      </c>
+      <c r="P89" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q89" s="74" t="s">
+        <v>324</v>
+      </c>
+      <c r="R89" s="131">
+        <v>201480</v>
+      </c>
+      <c r="S89" s="131">
+        <v>1000</v>
+      </c>
+      <c r="T89" s="131">
+        <v>1</v>
+      </c>
+      <c r="U89" s="131">
+        <v>1</v>
+      </c>
+      <c r="V89" s="74" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="91" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="92" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="93" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="94" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="95" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="96" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="97" ht="15.75" customHeight="1"/>
     <row r="98" ht="15.75" customHeight="1"/>
     <row r="99" ht="15.75" customHeight="1"/>
@@ -7072,8 +7197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y987"/>
   <sheetViews>
-    <sheetView topLeftCell="L64" workbookViewId="0">
-      <selection activeCell="U94" sqref="U94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9060,15 +9185,15 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="130"/>
-      <c r="B33" s="136" t="s">
+      <c r="A33" s="129"/>
+      <c r="B33" s="140" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="137"/>
-      <c r="D33" s="137"/>
-      <c r="E33" s="137"/>
-      <c r="F33" s="137"/>
-      <c r="G33" s="137"/>
+      <c r="C33" s="141"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="141"/>
+      <c r="F33" s="141"/>
+      <c r="G33" s="141"/>
       <c r="H33" s="59"/>
       <c r="I33" s="59"/>
       <c r="J33" s="59"/>
@@ -9908,17 +10033,17 @@
       </c>
     </row>
     <row r="48" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A48" s="130"/>
-      <c r="B48" s="138" t="s">
+      <c r="A48" s="129"/>
+      <c r="B48" s="142" t="s">
         <v>204</v>
       </c>
-      <c r="C48" s="139"/>
-      <c r="D48" s="139"/>
-      <c r="E48" s="139"/>
-      <c r="F48" s="139"/>
-      <c r="G48" s="139"/>
-      <c r="H48" s="139"/>
-      <c r="I48" s="139"/>
+      <c r="C48" s="143"/>
+      <c r="D48" s="143"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="143"/>
+      <c r="G48" s="143"/>
+      <c r="H48" s="143"/>
+      <c r="I48" s="143"/>
       <c r="J48" s="59"/>
       <c r="K48" s="59"/>
       <c r="L48" s="59"/>
@@ -10723,16 +10848,16 @@
       </c>
     </row>
     <row r="64" spans="1:22" s="101" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A64" s="131"/>
-      <c r="B64" s="135" t="s">
+      <c r="A64" s="130"/>
+      <c r="B64" s="139" t="s">
         <v>260</v>
       </c>
-      <c r="C64" s="135"/>
-      <c r="D64" s="135"/>
-      <c r="E64" s="135"/>
-      <c r="F64" s="135"/>
-      <c r="G64" s="135"/>
-      <c r="H64" s="135"/>
+      <c r="C64" s="139"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="139"/>
+      <c r="F64" s="139"/>
+      <c r="G64" s="139"/>
+      <c r="H64" s="139"/>
       <c r="T64" s="57" t="s">
         <v>201</v>
       </c>
@@ -12334,7 +12459,7 @@
         <v>1</v>
       </c>
       <c r="T90" s="57" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="U90" s="55" t="s">
         <v>324</v>
@@ -12343,8 +12468,69 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A91" s="1"/>
+    <row r="91" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A91" s="120" t="s">
+        <v>336</v>
+      </c>
+      <c r="B91" s="55"/>
+      <c r="C91" s="55"/>
+      <c r="D91" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="E91" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="F91" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="G91" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="H91" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="67">
+        <v>12230</v>
+      </c>
+      <c r="J91" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="K91" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="L91" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M91" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="N91" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="O91" s="67">
+        <v>100000000</v>
+      </c>
+      <c r="P91" s="55" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q91" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="R91" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S91" s="68" t="b">
+        <v>1</v>
+      </c>
+      <c r="T91" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="U91" s="55" t="s">
+        <v>324</v>
+      </c>
+      <c r="V91" s="67">
+        <v>201480</v>
+      </c>
     </row>
     <row r="92" spans="1:22" ht="15.75" customHeight="1">
       <c r="A92" s="1"/>
@@ -15050,7 +15236,7 @@
   <dimension ref="A1:R990"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65:N90"/>
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16659,14 +16845,14 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="73"/>
-      <c r="B33" s="140" t="s">
+      <c r="B33" s="144" t="s">
         <v>236</v>
       </c>
-      <c r="C33" s="140"/>
-      <c r="D33" s="140"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
+      <c r="C33" s="144"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="144"/>
+      <c r="G33" s="144"/>
       <c r="H33" s="57"/>
       <c r="I33" s="57"/>
       <c r="J33" s="57"/>
@@ -17358,14 +17544,14 @@
     </row>
     <row r="49" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A49" s="73"/>
-      <c r="B49" s="132" t="s">
+      <c r="B49" s="136" t="s">
         <v>235</v>
       </c>
-      <c r="C49" s="132"/>
-      <c r="D49" s="132"/>
-      <c r="E49" s="132"/>
-      <c r="F49" s="132"/>
-      <c r="G49" s="132"/>
+      <c r="C49" s="136"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="136"/>
       <c r="H49" s="57"/>
       <c r="I49" s="57"/>
       <c r="J49" s="57"/>
@@ -18027,15 +18213,15 @@
     </row>
     <row r="65" spans="1:18" s="101" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A65" s="102"/>
-      <c r="B65" s="135" t="s">
+      <c r="B65" s="139" t="s">
         <v>260</v>
       </c>
-      <c r="C65" s="135"/>
-      <c r="D65" s="135"/>
-      <c r="E65" s="135"/>
-      <c r="F65" s="135"/>
-      <c r="G65" s="135"/>
-      <c r="H65" s="135"/>
+      <c r="C65" s="139"/>
+      <c r="D65" s="139"/>
+      <c r="E65" s="139"/>
+      <c r="F65" s="139"/>
+      <c r="G65" s="139"/>
+      <c r="H65" s="139"/>
       <c r="N65" s="72" t="s">
         <v>201</v>
       </c>
@@ -19336,7 +19522,7 @@
         <v>65</v>
       </c>
       <c r="N91" s="54" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="O91" s="114" t="s">
         <v>61</v>
@@ -19351,25 +19537,57 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A92" s="119"/>
-      <c r="B92" s="55"/>
-      <c r="C92" s="55"/>
-      <c r="D92" s="55"/>
-      <c r="E92" s="55"/>
-      <c r="F92" s="105"/>
-      <c r="G92" s="105"/>
-      <c r="H92" s="55"/>
-      <c r="I92" s="55"/>
-      <c r="J92" s="77"/>
-      <c r="K92" s="53"/>
-      <c r="L92" s="53"/>
-      <c r="M92" s="71"/>
-      <c r="N92" s="72"/>
-      <c r="O92" s="55"/>
-      <c r="P92" s="55"/>
-      <c r="Q92" s="55"/>
-      <c r="R92" s="51"/>
+    <row r="92" spans="1:18" s="52" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A92" s="121" t="s">
+        <v>336</v>
+      </c>
+      <c r="B92" s="114"/>
+      <c r="C92" s="114"/>
+      <c r="D92" s="114" t="s">
+        <v>340</v>
+      </c>
+      <c r="E92" s="114" t="s">
+        <v>340</v>
+      </c>
+      <c r="F92" s="122" t="s">
+        <v>337</v>
+      </c>
+      <c r="G92" s="122" t="s">
+        <v>337</v>
+      </c>
+      <c r="H92" s="114" t="s">
+        <v>22</v>
+      </c>
+      <c r="I92" s="114" t="s">
+        <v>23</v>
+      </c>
+      <c r="J92" s="114" t="s">
+        <v>24</v>
+      </c>
+      <c r="K92" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="L92" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="M92" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="N92" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="O92" s="114" t="s">
+        <v>61</v>
+      </c>
+      <c r="P92" s="114" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q92" s="114" t="s">
+        <v>324</v>
+      </c>
+      <c r="R92" s="51">
+        <v>201480</v>
+      </c>
     </row>
     <row r="93" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A93" s="119"/>
@@ -23074,8 +23292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD982"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -24362,14 +24580,14 @@
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="59"/>
-      <c r="B33" s="132" t="s">
+      <c r="B33" s="136" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="133"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
-      <c r="G33" s="133"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
+      <c r="E33" s="137"/>
+      <c r="F33" s="137"/>
+      <c r="G33" s="137"/>
       <c r="H33" s="91" t="s">
         <v>201</v>
       </c>
@@ -24867,14 +25085,14 @@
     </row>
     <row r="47" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A47" s="59"/>
-      <c r="B47" s="132" t="s">
+      <c r="B47" s="136" t="s">
         <v>204</v>
       </c>
-      <c r="C47" s="133"/>
-      <c r="D47" s="133"/>
-      <c r="E47" s="133"/>
-      <c r="F47" s="133"/>
-      <c r="G47" s="133"/>
+      <c r="C47" s="137"/>
+      <c r="D47" s="137"/>
+      <c r="E47" s="137"/>
+      <c r="F47" s="137"/>
+      <c r="G47" s="137"/>
       <c r="H47" s="91" t="s">
         <v>201</v>
       </c>
@@ -25382,13 +25600,13 @@
     </row>
     <row r="63" spans="1:14" s="100" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A63" s="109"/>
-      <c r="B63" s="141" t="s">
+      <c r="B63" s="145" t="s">
         <v>260</v>
       </c>
-      <c r="C63" s="142"/>
-      <c r="D63" s="142"/>
-      <c r="E63" s="142"/>
-      <c r="F63" s="143"/>
+      <c r="C63" s="146"/>
+      <c r="D63" s="146"/>
+      <c r="E63" s="146"/>
+      <c r="F63" s="147"/>
       <c r="G63" s="110"/>
       <c r="H63" s="91" t="s">
         <v>201</v>
@@ -26378,7 +26596,7 @@
         <v>330</v>
       </c>
       <c r="H89" s="106" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="I89" s="107">
         <v>1</v>
@@ -26399,7 +26617,46 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A90" s="121" t="s">
+        <v>336</v>
+      </c>
+      <c r="B90" s="104"/>
+      <c r="C90" s="104"/>
+      <c r="D90" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="E90" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="F90" s="122" t="s">
+        <v>337</v>
+      </c>
+      <c r="G90" s="104" t="s">
+        <v>338</v>
+      </c>
+      <c r="H90" s="106" t="s">
+        <v>54</v>
+      </c>
+      <c r="I90" s="107">
+        <v>1</v>
+      </c>
+      <c r="J90" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="K90" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L90" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="M90" s="104" t="s">
+        <v>324</v>
+      </c>
+      <c r="N90" s="51">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="91" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="92" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="93" spans="1:14" ht="15.75" customHeight="1"/>

</xml_diff>